<commit_message>
Updated AIC comparison and got code ready to get example fit of 7 param model
</commit_message>
<xml_diff>
--- a/AIC comparison hp toolbox.xlsx
+++ b/AIC comparison hp toolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{727BE488-3010-4F12-A045-65B378C3F1F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43F210B-AD8F-4A59-B271-2B146CAC6F07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A472E74-28FF-4F20-915D-1A99B91A0647}"/>
   </bookViews>
@@ -31,12 +31,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>9 param</t>
   </si>
   <si>
     <t>7 param</t>
+  </si>
+  <si>
+    <t>Cell Line</t>
+  </si>
+  <si>
+    <t>HK-2</t>
+  </si>
+  <si>
+    <t>UMRC6</t>
+  </si>
+  <si>
+    <t>UOK262</t>
+  </si>
+  <si>
+    <t>UOK+DIDS</t>
+  </si>
+  <si>
+    <t>siRNA_c</t>
+  </si>
+  <si>
+    <t>siRNA</t>
+  </si>
+  <si>
+    <t>Pyruvate AIC Difference</t>
+  </si>
+  <si>
+    <t>Intracellular Lactate AIC Difference</t>
+  </si>
+  <si>
+    <t>Extracellular Lactate Difference</t>
   </si>
 </sst>
 </file>
@@ -391,7 +421,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:K23"/>
+      <selection activeCell="H1" sqref="H1:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,6 +433,18 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -423,6 +465,9 @@
       <c r="G2">
         <v>1654.8938869597118</v>
       </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
       <c r="I2">
         <f>A2-E2</f>
         <v>4.0000002766496436</v>
@@ -455,6 +500,9 @@
       <c r="G3">
         <v>1369.3170900420705</v>
       </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
       <c r="I3">
         <f t="shared" ref="I3:I23" si="1">A3-E3</f>
         <v>3.9981929143414163</v>
@@ -487,6 +535,9 @@
       <c r="G4">
         <v>1579.0832652976844</v>
       </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
       <c r="I4">
         <f t="shared" si="1"/>
         <v>3.9999827970041224</v>
@@ -519,6 +570,9 @@
       <c r="G5">
         <v>1884.9331066616555</v>
       </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
       <c r="I5">
         <f t="shared" si="1"/>
         <v>3.9969611633332534</v>
@@ -551,6 +605,9 @@
       <c r="G6">
         <v>1748.5421504869457</v>
       </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
       <c r="I6">
         <f t="shared" si="1"/>
         <v>4.000019656598397</v>
@@ -583,6 +640,9 @@
       <c r="G7">
         <v>1876.8313575376681</v>
       </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
       <c r="I7">
         <f t="shared" si="1"/>
         <v>4.0029358423003032</v>
@@ -615,6 +675,9 @@
       <c r="G8">
         <v>1673.6191375567414</v>
       </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
       <c r="I8">
         <f t="shared" si="1"/>
         <v>3.9993031654739752</v>
@@ -647,6 +710,9 @@
       <c r="G9">
         <v>1779.1941432769693</v>
       </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
       <c r="I9">
         <f t="shared" si="1"/>
         <v>3.9999970297835716</v>
@@ -679,6 +745,9 @@
       <c r="G10">
         <v>1629.4938427291459</v>
       </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
       <c r="I10">
         <f t="shared" si="1"/>
         <v>4.0000526641806573</v>
@@ -711,6 +780,9 @@
       <c r="G11">
         <v>1422.9671136278478</v>
       </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
       <c r="I11">
         <f t="shared" si="1"/>
         <v>4.0007260094639605</v>
@@ -743,6 +815,9 @@
       <c r="G12">
         <v>1401.2526586545646</v>
       </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
       <c r="I12">
         <f t="shared" si="1"/>
         <v>4.000910419725642</v>
@@ -775,6 +850,9 @@
       <c r="G13">
         <v>1869.1465558948457</v>
       </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
       <c r="I13">
         <f t="shared" si="1"/>
         <v>3.999999576682967</v>
@@ -807,6 +885,9 @@
       <c r="G14">
         <v>1759.5967950965151</v>
       </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
       <c r="I14">
         <f t="shared" si="1"/>
         <v>4.015241254139255</v>
@@ -839,6 +920,9 @@
       <c r="G15">
         <v>1750.5472354606577</v>
       </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
       <c r="I15">
         <f t="shared" si="1"/>
         <v>3.9940320247860654</v>
@@ -871,6 +955,9 @@
       <c r="G16">
         <v>1832.001306978955</v>
       </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
       <c r="I16">
         <f t="shared" si="1"/>
         <v>3.9248720031146149</v>
@@ -903,6 +990,9 @@
       <c r="G17">
         <v>1549.3439003568135</v>
       </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
       <c r="I17">
         <f t="shared" si="1"/>
         <v>3.9999343886952374</v>
@@ -935,6 +1025,9 @@
       <c r="G18">
         <v>1694.6493438790021</v>
       </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
       <c r="I18">
         <f t="shared" si="1"/>
         <v>4.012270364682081</v>
@@ -967,6 +1060,9 @@
       <c r="G19">
         <v>2071.8516997418374</v>
       </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
       <c r="I19">
         <f t="shared" si="1"/>
         <v>4.2084745843808378</v>
@@ -999,6 +1095,9 @@
       <c r="G20">
         <v>1975.0688096723513</v>
       </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
       <c r="I20">
         <f t="shared" si="1"/>
         <v>3.9997509923591679</v>
@@ -1031,6 +1130,9 @@
       <c r="G21">
         <v>1871.125556341239</v>
       </c>
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
       <c r="I21">
         <f t="shared" si="1"/>
         <v>4.0094703363170083</v>
@@ -1063,6 +1165,9 @@
       <c r="G22">
         <v>1975.0244367991929</v>
       </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
       <c r="I22">
         <f t="shared" si="1"/>
         <v>4.0006858837436994</v>
@@ -1094,6 +1199,9 @@
       </c>
       <c r="G23">
         <v>1725.7631208362495</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>

</xml_diff>